<commit_message>
Actualización de valores tabla
</commit_message>
<xml_diff>
--- a/Prueba Mockup02.xlsx
+++ b/Prueba Mockup02.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.lozano\Documents\JorgeLozano\Datos JL\Personal\Cursos\Sensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorge.lozano\SystemDevelopment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5100E666-A6E9-4967-801F-1DD289DB9A3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07423988-E70C-4025-9B3D-A1CD3DF4A70B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{87A87D5D-CA78-4F5B-8C31-8BADD7D9B1AE}"/>
   </bookViews>
@@ -523,7 +523,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE31130-D34C-45F3-A5F0-C9C8CAB5FE47}">
   <dimension ref="A1:R91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -618,7 +620,7 @@
         <v>23</v>
       </c>
       <c r="F2" s="5">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G2" s="5">
         <v>1</v>
@@ -674,7 +676,7 @@
         <v>41</v>
       </c>
       <c r="F3" s="6">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>

</xml_diff>